<commit_message>
dynamic notification times and values from spreadsheet
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
     <sheet name="Setup" sheetId="2" r:id="rId2"/>
     <sheet name="stationsLearn" sheetId="3" r:id="rId3"/>
     <sheet name="stationsExperiment" sheetId="4" r:id="rId4"/>
+    <sheet name="interruptionsLearn" sheetId="5" r:id="rId5"/>
+    <sheet name="interruptionsExperiment" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Time</t>
   </si>
@@ -121,6 +123,12 @@
   </si>
   <si>
     <t>Kitty Cat 6</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -176,8 +184,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -199,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -208,6 +218,7 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -216,6 +227,7 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -804,9 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -1069,6 +1079,103 @@
       </c>
       <c r="I9">
         <v>645</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>20000</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>40000</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>60000</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>80000</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>120000</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minutes and seconds, different pages for AMT and Lab
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="stationsExperiment" sheetId="4" r:id="rId4"/>
     <sheet name="interruptionsLearn" sheetId="5" r:id="rId5"/>
     <sheet name="interruptionsExperiment" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Time</t>
   </si>
@@ -129,6 +130,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time </t>
   </si>
 </sst>
 </file>
@@ -184,8 +188,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -219,6 +249,19 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -228,6 +271,19 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,7 +736,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -725,7 +781,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -754,7 +810,7 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -783,7 +839,7 @@
         <v>59</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -814,9 +870,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -860,7 +918,7 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -889,7 +947,7 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -918,7 +976,7 @@
         <v>100</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -947,7 +1005,7 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -976,7 +1034,7 @@
         <v>50</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1005,7 +1063,7 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1021,64 +1079,6 @@
       </c>
       <c r="I7">
         <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8">
-        <v>410</v>
-      </c>
-      <c r="I8">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9">
-        <v>410</v>
-      </c>
-      <c r="I9">
-        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -1096,7 +1096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1122,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E1" sqref="E1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1139,43 +1139,382 @@
       </c>
     </row>
     <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>34944</v>
+      </c>
+      <c r="B2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>61565</v>
+      </c>
+      <c r="B3" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>90225</v>
+      </c>
+      <c r="B4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>126138</v>
+      </c>
+      <c r="B5" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>154224</v>
+      </c>
+      <c r="B6" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>181116</v>
+      </c>
+      <c r="B7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>219996</v>
+      </c>
+      <c r="B8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>241418</v>
+      </c>
+      <c r="B9" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>272938</v>
+      </c>
+      <c r="B10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1">
+        <v>30000</v>
+      </c>
+      <c r="B1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <f ca="1">10000*RAND()</f>
+        <v>8554.9128958103247</v>
+      </c>
+      <c r="E1">
+        <f ca="1">FLOOR(A1+D1,1)</f>
+        <v>38554</v>
+      </c>
+      <c r="F1" t="b">
+        <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <f>A1/60000</f>
+        <v>0.5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
-        <v>20000</v>
+        <v>60000</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f ca="1">10000*RAND()</f>
+        <v>2292.9921806122188</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:E9" ca="1" si="0">FLOOR(A2+D2,1)</f>
+        <v>62292</v>
+      </c>
+      <c r="F2" t="b">
+        <f t="shared" ref="F2:F9" ca="1" si="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>A2/60000</f>
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>126138</v>
+      </c>
+      <c r="K2" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
-        <v>40000</v>
+        <v>90000</v>
       </c>
       <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D9" ca="1" si="2">10000*RAND()</f>
+        <v>1934.0933301370544</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>91934</v>
+      </c>
+      <c r="F3" t="b">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <f>A3/60000</f>
+        <v>1.5</v>
+      </c>
+      <c r="J3" s="1">
+        <v>219996</v>
+      </c>
+      <c r="K3" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:11">
       <c r="A4">
-        <v>60000</v>
+        <v>120000</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="2"/>
+        <v>5379.1285385027868</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>125379</v>
+      </c>
+      <c r="F4" t="b">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>A4/60000</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
-        <v>80000</v>
+        <v>150000</v>
       </c>
       <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="2"/>
+        <v>5756.2818325731414</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>155756</v>
+      </c>
+      <c r="F5" t="b">
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="G5">
+        <f>A5/60000</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
-        <v>120000</v>
+        <v>180000</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="2"/>
+        <v>573.73057830586549</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>180573</v>
+      </c>
+      <c r="F6" t="b">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <f>A6/60000</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>210000</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="2"/>
+        <v>722.31808169150429</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>210722</v>
+      </c>
+      <c r="F7" t="b">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>A7/60000</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>240000</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="2"/>
+        <v>8167.3280593117388</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>248167</v>
+      </c>
+      <c r="F8" t="b">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>A8/60000</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>270000</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="2"/>
+        <v>3923.3235948907932</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>273923</v>
+      </c>
+      <c r="F9" t="b">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>A9/60000</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15">
+        <v>410</v>
+      </c>
+      <c r="J15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16">
+        <v>410</v>
+      </c>
+      <c r="J16">
+        <v>645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
swipesy seems to work well now
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>Time</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">time </t>
+  </si>
+  <si>
+    <t>swipesyCount</t>
   </si>
 </sst>
 </file>
@@ -188,8 +191,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -239,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -262,6 +267,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -284,6 +290,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -872,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1094,24 +1101,28 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1122,92 +1133,122 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>34944</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>61565</v>
       </c>
       <c r="B3" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>90225</v>
       </c>
       <c r="B4" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>126138</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>154224</v>
       </c>
       <c r="B6" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>181116</v>
       </c>
       <c r="B7" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>219996</v>
       </c>
       <c r="B8" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>241418</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>272938</v>
       </c>
       <c r="B10" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1240,18 +1281,18 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>8554.9128958103247</v>
+        <v>8582.384526044123</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>38554</v>
+        <v>38582</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="G1">
-        <f>A1/60000</f>
+        <f t="shared" ref="G1:G9" si="0">A1/60000</f>
         <v>0.5</v>
       </c>
       <c r="J1" t="s">
@@ -1270,18 +1311,18 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>2292.9921806122188</v>
+        <v>1630.2155855266321</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E9" ca="1" si="0">FLOOR(A2+D2,1)</f>
-        <v>62292</v>
+        <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
+        <v>61630</v>
       </c>
       <c r="F2" t="b">
-        <f t="shared" ref="F2:F9" ca="1" si="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
+        <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>A2/60000</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J2" s="1">
@@ -1299,19 +1340,19 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" ca="1" si="2">10000*RAND()</f>
-        <v>1934.0933301370544</v>
+        <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
+        <v>3303.1982506058675</v>
       </c>
       <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>91934</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>93303</v>
       </c>
       <c r="F3" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f>A3/60000</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="J3" s="1">
@@ -1329,19 +1370,19 @@
         <v>0</v>
       </c>
       <c r="D4">
+        <f t="shared" ca="1" si="3"/>
+        <v>8136.9511396677108</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="1"/>
+        <v>128136</v>
+      </c>
+      <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>5379.1285385027868</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>125379</v>
-      </c>
-      <c r="F4" t="b">
-        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f>A4/60000</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1353,19 +1394,19 @@
         <v>1</v>
       </c>
       <c r="D5">
+        <f t="shared" ca="1" si="3"/>
+        <v>987.18182263501262</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>150987</v>
+      </c>
+      <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>5756.2818325731414</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>155756</v>
-      </c>
-      <c r="F5" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <f>A5/60000</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -1377,19 +1418,19 @@
         <v>1</v>
       </c>
       <c r="D6">
+        <f t="shared" ca="1" si="3"/>
+        <v>6662.2576393975287</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>186662</v>
+      </c>
+      <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>573.73057830586549</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ca="1" si="0"/>
-        <v>180573</v>
-      </c>
-      <c r="F6" t="b">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G6">
-        <f>A6/60000</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1401,19 +1442,19 @@
         <v>0</v>
       </c>
       <c r="D7">
+        <f t="shared" ca="1" si="3"/>
+        <v>4652.9263659403832</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>214652</v>
+      </c>
+      <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>722.31808169150429</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>210722</v>
-      </c>
-      <c r="F7" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <f>A7/60000</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -1422,19 +1463,19 @@
         <v>240000</v>
       </c>
       <c r="D8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2833.3824954270672</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>242833</v>
+      </c>
+      <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>8167.3280593117388</v>
-      </c>
-      <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>248167</v>
-      </c>
-      <c r="F8" t="b">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <f>A8/60000</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1443,19 +1484,19 @@
         <v>270000</v>
       </c>
       <c r="D9">
+        <f t="shared" ca="1" si="3"/>
+        <v>8947.9565614125513</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>278947</v>
+      </c>
+      <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>3923.3235948907932</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ca="1" si="0"/>
-        <v>273923</v>
-      </c>
-      <c r="F9" t="b">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f>A9/60000</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added custom watch face, moved agreement window over and fixed some niggly problems
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="37500" yWindow="1720" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -102,24 +102,12 @@
     <t>leftOffset</t>
   </si>
   <si>
-    <t>Kitty Cat 1</t>
-  </si>
-  <si>
     <t>block_number</t>
   </si>
   <si>
     <t>station_id</t>
   </si>
   <si>
-    <t>Kitty Cat 2</t>
-  </si>
-  <si>
-    <t>Kitty Cat 3</t>
-  </si>
-  <si>
-    <t>Kitty Cat 4</t>
-  </si>
-  <si>
     <t>Kitty Cat 5</t>
   </si>
   <si>
@@ -178,6 +166,18 @@
   </si>
   <si>
     <t>swipesyDuration</t>
+  </si>
+  <si>
+    <t>Pet 1</t>
+  </si>
+  <si>
+    <t>Pet 2</t>
+  </si>
+  <si>
+    <t>Pet 3</t>
+  </si>
+  <si>
+    <t>Pet 4</t>
   </si>
 </sst>
 </file>
@@ -233,8 +233,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -314,7 +320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -352,6 +358,9 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -389,6 +398,9 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -840,18 +852,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -886,7 +898,7 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -894,8 +906,8 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>25</v>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="H2">
         <v>60</v>
@@ -915,7 +927,7 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -923,8 +935,8 @@
       <c r="F3">
         <v>4</v>
       </c>
-      <c r="G3" t="s">
-        <v>28</v>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="H3">
         <v>60</v>
@@ -952,8 +964,8 @@
       <c r="F4">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
-        <v>29</v>
+      <c r="G4" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="H4">
         <v>60</v>
@@ -978,17 +990,17 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G4" sqref="G4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -1023,7 +1035,7 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -1032,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H2">
         <v>60</v>
@@ -1052,7 +1064,7 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1061,7 +1073,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>60</v>
@@ -1081,16 +1093,16 @@
         <v>100</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H4">
         <v>60</v>
@@ -1110,7 +1122,7 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1119,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="H5">
         <v>60</v>
@@ -1139,7 +1151,7 @@
         <v>50</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1148,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="H6">
         <v>60</v>
@@ -1168,7 +1180,7 @@
         <v>100</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1177,7 +1189,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H7">
         <v>410</v>
@@ -1209,13 +1221,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N3" sqref="N3:N19"/>
     </sheetView>
   </sheetViews>
@@ -1244,19 +1256,19 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1268,22 +1280,22 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
         <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1303,22 +1315,22 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>43</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
-        <v>47</v>
       </c>
       <c r="L2">
         <v>600000</v>
@@ -1353,16 +1365,16 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
         <v>43</v>
-      </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>47</v>
       </c>
       <c r="L3">
         <v>600000</v>
@@ -1391,22 +1403,22 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>43</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
       </c>
       <c r="L4">
         <v>600000</v>
@@ -1441,16 +1453,16 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
         <v>43</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>47</v>
       </c>
       <c r="L5">
         <v>600000</v>
@@ -1485,16 +1497,16 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
         <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" t="s">
-        <v>47</v>
       </c>
       <c r="L6">
         <v>600000</v>
@@ -1523,22 +1535,22 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
         <v>41</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>43</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>47</v>
       </c>
       <c r="L7">
         <v>600000</v>
@@ -1573,16 +1585,16 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
         <v>43</v>
-      </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
       </c>
       <c r="L8">
         <v>600000</v>
@@ -1617,16 +1629,16 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" t="s">
         <v>43</v>
-      </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
       </c>
       <c r="L9">
         <v>600000</v>
@@ -1655,22 +1667,22 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
       </c>
       <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
         <v>41</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>43</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>47</v>
       </c>
       <c r="L10">
         <v>600000</v>
@@ -1702,16 +1714,16 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
         <v>41</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>43</v>
-      </c>
-      <c r="J11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" t="s">
-        <v>47</v>
       </c>
       <c r="L11">
         <v>600000</v>
@@ -1743,16 +1755,16 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" t="s">
         <v>43</v>
-      </c>
-      <c r="J12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" t="s">
-        <v>47</v>
       </c>
       <c r="L12">
         <v>600000</v>
@@ -1784,16 +1796,16 @@
         <v>6</v>
       </c>
       <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
         <v>41</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>43</v>
-      </c>
-      <c r="J13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" t="s">
-        <v>47</v>
       </c>
       <c r="L13">
         <v>600000</v>
@@ -1825,16 +1837,16 @@
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" t="s">
         <v>43</v>
-      </c>
-      <c r="J14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" t="s">
-        <v>47</v>
       </c>
       <c r="L14">
         <v>600000</v>
@@ -1866,16 +1878,16 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" t="s">
         <v>43</v>
-      </c>
-      <c r="J15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" t="s">
-        <v>47</v>
       </c>
       <c r="L15">
         <v>600000</v>
@@ -1907,16 +1919,16 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
         <v>41</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>43</v>
-      </c>
-      <c r="J16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" t="s">
-        <v>47</v>
       </c>
       <c r="L16">
         <v>600000</v>
@@ -1948,16 +1960,16 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
         <v>43</v>
-      </c>
-      <c r="J17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" t="s">
-        <v>47</v>
       </c>
       <c r="L17">
         <v>600000</v>
@@ -1989,16 +2001,16 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
         <v>43</v>
-      </c>
-      <c r="J18" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" t="s">
-        <v>47</v>
       </c>
       <c r="L18">
         <v>600000</v>
@@ -2030,16 +2042,16 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" t="s">
         <v>41</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>43</v>
-      </c>
-      <c r="J19" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" t="s">
-        <v>47</v>
       </c>
       <c r="L19">
         <v>600000</v>
@@ -2098,25 +2110,25 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>4145.0731326070463</v>
+        <v>1118.4146586467748</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>34145</v>
+        <v>31118</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:G9" si="0">A1/60000</f>
         <v>0.5</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2128,11 +2140,11 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>9655.4875804915755</v>
+        <v>2257.8906356028106</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>69655</v>
+        <v>62257</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
@@ -2158,11 +2170,11 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>5575.4969217900725</v>
+        <v>1991.6256852309289</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>95575</v>
+        <v>91991</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2188,15 +2200,15 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>998.88365119612081</v>
+        <v>6101.3244194583258</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>120998</v>
+        <v>126101</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -2212,15 +2224,15 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>1963.777691876305</v>
+        <v>982.68089160964519</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>151963</v>
+        <v>150982</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -2236,15 +2248,15 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>9430.5562846782141</v>
+        <v>7960.3464346830442</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>189430</v>
+        <v>187960</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -2260,11 +2272,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>3536.2969647756981</v>
+        <v>1421.6689857306465</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>213536</v>
+        <v>211421</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2281,11 +2293,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>7258.6985073136602</v>
+        <v>4494.9420200599998</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>247258</v>
+        <v>244494</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2302,15 +2314,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>7312.6028634418781</v>
+        <v>5056.6082665003187</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>277312</v>
+        <v>275056</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -2337,7 +2349,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I15">
         <v>410</v>
@@ -2366,7 +2378,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I16">
         <v>410</v>

</xml_diff>

<commit_message>
fixed CSS issues on the smartwatch screen and the station layout
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="37500" yWindow="1720" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -852,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1192,7 +1192,7 @@
         <v>50</v>
       </c>
       <c r="H7">
-        <v>410</v>
+        <v>350</v>
       </c>
       <c r="I7">
         <v>35</v>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N19"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2110,15 +2110,15 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>1118.4146586467748</v>
+        <v>126.10527656682468</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>31118</v>
+        <v>30126</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:G9" si="0">A1/60000</f>
@@ -2140,15 +2140,15 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>2257.8906356028106</v>
+        <v>2428.8739512957227</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>62257</v>
+        <v>62428</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
@@ -2170,11 +2170,11 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>1991.6256852309289</v>
+        <v>9590.3563739520832</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>91991</v>
+        <v>99590</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2200,11 +2200,11 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>6101.3244194583258</v>
+        <v>4219.3225989863186</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>126101</v>
+        <v>124219</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2224,11 +2224,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>982.68089160964519</v>
+        <v>5564.945428223431</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>150982</v>
+        <v>155564</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2248,11 +2248,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>7960.3464346830442</v>
+        <v>1894.4921455238784</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>187960</v>
+        <v>181894</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2272,11 +2272,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>1421.6689857306465</v>
+        <v>5795.0450084879258</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>211421</v>
+        <v>215795</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2293,11 +2293,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>4494.9420200599998</v>
+        <v>6083.2121591525774</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>244494</v>
+        <v>246083</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2314,11 +2314,11 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>5056.6082665003187</v>
+        <v>1805.426513362477</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>275056</v>
+        <v>271805</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>

</xml_diff>

<commit_message>
formatting tweaks to the pet position in the view
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -990,7 +990,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1148,7 +1148,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1246,7 +1246,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2110,11 +2110,11 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>126.10527656682468</v>
+        <v>9598.7447933757994</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>30126</v>
+        <v>39598</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
@@ -2140,11 +2140,11 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>2428.8739512957227</v>
+        <v>9678.2429064708158</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>62428</v>
+        <v>69678</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
@@ -2170,15 +2170,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>9590.3563739520832</v>
+        <v>7660.1779285482371</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>99590</v>
+        <v>97660</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -2200,11 +2200,11 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>4219.3225989863186</v>
+        <v>4923.714279953123</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>124219</v>
+        <v>124923</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2224,11 +2224,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>5564.945428223431</v>
+        <v>6815.3165990807665</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>155564</v>
+        <v>156815</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2248,11 +2248,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>1894.4921455238784</v>
+        <v>5296.3467241353064</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>181894</v>
+        <v>185296</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2272,11 +2272,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>5795.0450084879258</v>
+        <v>5597.5695709677229</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>215795</v>
+        <v>215597</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2293,11 +2293,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>6083.2121591525774</v>
+        <v>8838.9471699769401</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>246083</v>
+        <v>248838</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2314,15 +2314,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>1805.426513362477</v>
+        <v>592.10752493874975</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>271805</v>
+        <v>270592</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
fixed erroneous text on valid message
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="51">
   <si>
     <t>Time</t>
   </si>
@@ -233,8 +233,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -320,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -361,6 +365,8 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -401,6 +407,8 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -989,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1243,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2068,17 +2076,44 @@
         <v>0</v>
       </c>
       <c r="B20" s="1">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="C20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L20">
+        <v>600000</v>
+      </c>
+      <c r="M20">
+        <v>30000</v>
+      </c>
+      <c r="N20">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2110,15 +2145,15 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>9598.7447933757994</v>
+        <v>6281.0597681597355</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>39598</v>
+        <v>36281</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:G9" si="0">A1/60000</f>
@@ -2140,15 +2175,15 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>9678.2429064708158</v>
+        <v>8445.5182331229244</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>69678</v>
+        <v>68445</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
@@ -2170,15 +2205,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>7660.1779285482371</v>
+        <v>7702.793435723961</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>97660</v>
+        <v>97702</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -2200,11 +2235,11 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>4923.714279953123</v>
+        <v>7641.0674646054276</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>124923</v>
+        <v>127641</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2224,11 +2259,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>6815.3165990807665</v>
+        <v>8001.4382053665531</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>156815</v>
+        <v>158001</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2248,11 +2283,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>5296.3467241353064</v>
+        <v>7679.4246900628114</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>185296</v>
+        <v>187679</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2272,11 +2307,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>5597.5695709677229</v>
+        <v>802.88680161735408</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>215597</v>
+        <v>210802</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2293,11 +2328,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>8838.9471699769401</v>
+        <v>2508.2704391787893</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>248838</v>
+        <v>242508</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2314,15 +2349,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>592.10752493874975</v>
+        <v>7271.2527895641588</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>270592</v>
+        <v>277271</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
game score delta amounts worked, and slower health reduction 6 to 4
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="50">
   <si>
     <t>Time</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>station_noise</t>
-  </si>
-  <si>
-    <t>view_cost</t>
   </si>
   <si>
     <t>id</t>
@@ -858,20 +855,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -891,11 +888,8 @@
       <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -911,20 +905,17 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>47</v>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
       </c>
       <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -940,20 +931,17 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>48</v>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3">
         <v>340</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1</v>
       </c>
@@ -964,21 +952,18 @@
         <v>59</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>49</v>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
       </c>
       <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="I4">
         <v>645</v>
       </c>
     </row>
@@ -995,20 +980,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -1028,11 +1013,8 @@
       <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1048,20 +1030,17 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2">
+        <v>60</v>
       </c>
       <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1072,25 +1051,22 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>60</v>
-      </c>
-      <c r="I3">
         <v>340</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1101,25 +1077,22 @@
         <v>100</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
       </c>
       <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="I4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1130,25 +1103,22 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
       </c>
       <c r="H5">
-        <v>60</v>
-      </c>
-      <c r="I5">
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1164,20 +1134,17 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6">
+        <v>60</v>
       </c>
       <c r="H6">
-        <v>60</v>
-      </c>
-      <c r="I6">
         <v>645</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1193,16 +1160,13 @@
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>50</v>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7">
+        <v>350</v>
       </c>
       <c r="H7">
-        <v>350</v>
-      </c>
-      <c r="I7">
         <v>35</v>
       </c>
     </row>
@@ -1229,13 +1193,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1264,19 +1228,19 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -1288,22 +1252,22 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1323,22 +1287,22 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L2">
         <v>600000</v>
@@ -1373,16 +1337,16 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L3">
         <v>600000</v>
@@ -1411,22 +1375,22 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4">
         <v>600000</v>
@@ -1461,16 +1425,16 @@
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L5">
         <v>600000</v>
@@ -1505,16 +1469,16 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6">
         <v>600000</v>
@@ -1543,22 +1507,22 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7">
         <v>600000</v>
@@ -1593,16 +1557,16 @@
         <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8">
         <v>600000</v>
@@ -1637,16 +1601,16 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>600000</v>
@@ -1675,22 +1639,22 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10">
         <v>600000</v>
@@ -1722,16 +1686,16 @@
         <v>6</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11">
         <v>600000</v>
@@ -1763,16 +1727,16 @@
         <v>6</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L12">
         <v>600000</v>
@@ -1804,16 +1768,16 @@
         <v>6</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L13">
         <v>600000</v>
@@ -1845,16 +1809,16 @@
         <v>6</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L14">
         <v>600000</v>
@@ -1886,16 +1850,16 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L15">
         <v>600000</v>
@@ -1927,16 +1891,16 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L16">
         <v>600000</v>
@@ -1968,16 +1932,16 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L17">
         <v>600000</v>
@@ -2009,16 +1973,16 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L18">
         <v>600000</v>
@@ -2050,16 +2014,16 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L19">
         <v>600000</v>
@@ -2091,16 +2055,16 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L20">
         <v>600000</v>
@@ -2145,25 +2109,25 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>6281.0597681597355</v>
+        <v>9746.2717104225285</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>36281</v>
+        <v>39746</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:G9" si="0">A1/60000</f>
         <v>0.5</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2175,15 +2139,15 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>8445.5182331229244</v>
+        <v>5500.4488306660678</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>68445</v>
+        <v>65500</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
@@ -2205,11 +2169,11 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>7702.793435723961</v>
+        <v>8115.5066953677106</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>97702</v>
+        <v>98115</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2235,11 +2199,11 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>7641.0674646054276</v>
+        <v>4770.7554553551709</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>127641</v>
+        <v>124770</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2259,15 +2223,15 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>8001.4382053665531</v>
+        <v>1131.7236023534472</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>158001</v>
+        <v>151131</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -2283,11 +2247,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>7679.4246900628114</v>
+        <v>9170.8425389655731</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>187679</v>
+        <v>189170</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2307,11 +2271,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>802.88680161735408</v>
+        <v>5070.1166726409911</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>210802</v>
+        <v>215070</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2328,15 +2292,15 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>2508.2704391787893</v>
+        <v>3851.6020390350582</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>242508</v>
+        <v>243851</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -2349,15 +2313,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>7271.2527895641588</v>
+        <v>4913.2697498550315</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>277271</v>
+        <v>274913</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -2384,7 +2348,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15">
         <v>410</v>
@@ -2413,7 +2377,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16">
         <v>410</v>

</xml_diff>

<commit_message>
start healths to 100%
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -949,7 +949,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -982,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2109,15 +2109,15 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>9746.2717104225285</v>
+        <v>8824.779765116311</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>39746</v>
+        <v>38824</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:G9" si="0">A1/60000</f>
@@ -2139,15 +2139,15 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>5500.4488306660678</v>
+        <v>5717.1897499719207</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>65500</v>
+        <v>65717</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
@@ -2169,15 +2169,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>8115.5066953677106</v>
+        <v>2469.2354305888475</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>98115</v>
+        <v>92469</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -2199,11 +2199,11 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>4770.7554553551709</v>
+        <v>1252.187722188366</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>124770</v>
+        <v>121252</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2223,11 +2223,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>1131.7236023534472</v>
+        <v>6046.9665034828404</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>151131</v>
+        <v>156046</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2247,11 +2247,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>9170.8425389655731</v>
+        <v>3604.9283747672334</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>189170</v>
+        <v>183604</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2271,11 +2271,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>5070.1166726409911</v>
+        <v>3348.0832689370277</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>215070</v>
+        <v>213348</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2292,11 +2292,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>3851.6020390350582</v>
+        <v>6763.8173573265585</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>243851</v>
+        <v>246763</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2313,11 +2313,11 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>4913.2697498550315</v>
+        <v>9665.1007112294756</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>274913</v>
+        <v>279665</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>

</xml_diff>

<commit_message>
limit score to 0-100%, removed interrupt on condition 2
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="50">
   <si>
     <t>Time</t>
   </si>
@@ -857,7 +857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1217,12 +1217,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="6" max="6" width="27.5" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2039,42 +2040,8 @@
       <c r="A20">
         <v>0</v>
       </c>
-      <c r="B20" s="1">
-        <v>20000</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="G20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K20" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20">
-        <v>600000</v>
-      </c>
-      <c r="M20">
-        <v>30000</v>
-      </c>
-      <c r="N20">
-        <v>10000</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:14">
       <c r="B21" s="1"/>
@@ -2109,11 +2076,11 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>8824.779765116311</v>
+        <v>5841.9132789087316</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>38824</v>
+        <v>35841</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
@@ -2139,11 +2106,11 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>5717.1897499719207</v>
+        <v>1530.3880036453188</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>65717</v>
+        <v>61530</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
@@ -2169,15 +2136,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>2469.2354305888475</v>
+        <v>308.64286863622635</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>92469</v>
+        <v>90308</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -2199,15 +2166,15 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>1252.187722188366</v>
+        <v>9622.2941040839123</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>121252</v>
+        <v>129622</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -2223,11 +2190,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>6046.9665034828404</v>
+        <v>8175.5409368584187</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>156046</v>
+        <v>158175</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2247,11 +2214,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>3604.9283747672334</v>
+        <v>2974.6546511591755</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>183604</v>
+        <v>182974</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2271,11 +2238,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>3348.0832689370277</v>
+        <v>5831.9184396129531</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>213348</v>
+        <v>215831</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2292,15 +2259,15 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>6763.8173573265585</v>
+        <v>5002.4778434707005</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>246763</v>
+        <v>245002</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -2313,15 +2280,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>9665.1007112294756</v>
+        <v>5097.2836700549797</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>279665</v>
+        <v>275097</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
scroll stopped in experiment block, showseession fixes
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2076,15 +2076,15 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>5841.9132789087316</v>
+        <v>6819.0499941815888</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>35841</v>
+        <v>36819</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1">
         <f t="shared" ref="G1:G9" si="0">A1/60000</f>
@@ -2106,15 +2106,15 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>1530.3880036453188</v>
+        <v>5340.8662469037472</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>61530</v>
+        <v>65340</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
@@ -2136,15 +2136,15 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>308.64286863622635</v>
+        <v>8439.2582179115634</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>90308</v>
+        <v>98439</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -2166,15 +2166,15 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>9622.2941040839123</v>
+        <v>6455.5939892342431</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>129622</v>
+        <v>126455</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -2190,11 +2190,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>8175.5409368584187</v>
+        <v>5806.237007720506</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>158175</v>
+        <v>155806</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2214,11 +2214,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>2974.6546511591755</v>
+        <v>9973.6573303050609</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>182974</v>
+        <v>189973</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2238,15 +2238,15 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>5831.9184396129531</v>
+        <v>84.939839197738507</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>215831</v>
+        <v>210084</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -2259,15 +2259,15 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>5002.4778434707005</v>
+        <v>4608.6720808006266</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>245002</v>
+        <v>244608</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -2280,15 +2280,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>5097.2836700549797</v>
+        <v>4443.397201477982</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>275097</v>
+        <v>274443</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
moved back to 6 stations, still testing
</commit_message>
<xml_diff>
--- a/experiment_setup.xlsx
+++ b/experiment_setup.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notifications" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="52">
   <si>
     <t>Time</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>Pet 4</t>
+  </si>
+  <si>
+    <t>Pet 5</t>
+  </si>
+  <si>
+    <t>Pet 6</t>
   </si>
 </sst>
 </file>
@@ -230,8 +236,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -364,6 +380,11 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -406,6 +427,11 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -980,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1068,7 +1094,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1094,7 +1120,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1120,7 +1146,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1146,7 +1172,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1168,6 +1194,162 @@
       </c>
       <c r="H7">
         <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <v>350</v>
+      </c>
+      <c r="H11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="1">
+        <v>350</v>
+      </c>
+      <c r="H12">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="1">
+        <v>350</v>
+      </c>
+      <c r="H13">
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -1217,7 +1399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -2076,11 +2258,11 @@
       </c>
       <c r="D1">
         <f ca="1">10000*RAND()</f>
-        <v>6819.0499941815888</v>
+        <v>5026.8448271056777</v>
       </c>
       <c r="E1">
         <f ca="1">FLOOR(A1+D1,1)</f>
-        <v>36819</v>
+        <v>35026</v>
       </c>
       <c r="F1" t="b">
         <f ca="1">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
@@ -2106,15 +2288,15 @@
       </c>
       <c r="D2">
         <f ca="1">10000*RAND()</f>
-        <v>5340.8662469037472</v>
+        <v>7281.3382273689176</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E9" ca="1" si="1">FLOOR(A2+D2,1)</f>
-        <v>65340</v>
+        <v>67281</v>
       </c>
       <c r="F2" t="b">
         <f t="shared" ref="F2:F9" ca="1" si="2">IF(RAND()&gt;0.5,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
@@ -2136,11 +2318,11 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D9" ca="1" si="3">10000*RAND()</f>
-        <v>8439.2582179115634</v>
+        <v>1264.737817301964</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
-        <v>98439</v>
+        <v>91264</v>
       </c>
       <c r="F3" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2166,15 +2348,15 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="3"/>
-        <v>6455.5939892342431</v>
+        <v>8711.1596703550349</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>126455</v>
+        <v>128711</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -2190,11 +2372,11 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="3"/>
-        <v>5806.237007720506</v>
+        <v>8839.4986538654557</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>155806</v>
+        <v>158839</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2214,11 +2396,11 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="3"/>
-        <v>9973.6573303050609</v>
+        <v>2587.9354944795919</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>189973</v>
+        <v>182587</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2238,11 +2420,11 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="3"/>
-        <v>84.939839197738507</v>
+        <v>5390.8152687267811</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>210084</v>
+        <v>215390</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2259,11 +2441,11 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="3"/>
-        <v>4608.6720808006266</v>
+        <v>5466.876516587633</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>244608</v>
+        <v>245466</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" ca="1" si="2"/>
@@ -2280,15 +2462,15 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="3"/>
-        <v>4443.397201477982</v>
+        <v>5191.7234152494375</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>274443</v>
+        <v>275191</v>
       </c>
       <c r="F9" t="b">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>

</xml_diff>